<commit_message>
Added Week 8 Forecasts
</commit_message>
<xml_diff>
--- a/NFL2016/Weekly Forecasts/Week7.xlsx
+++ b/NFL2016/Weekly Forecasts/Week7.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="48">
   <si>
     <t>Chance of Winning</t>
   </si>
@@ -84,97 +84,85 @@
     <t>95th Percentile Score</t>
   </si>
   <si>
+    <t>Titans</t>
+  </si>
+  <si>
+    <t>Jaguars</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>Bengals</t>
+  </si>
+  <si>
+    <t>Washington</t>
+  </si>
+  <si>
+    <t>Colts</t>
+  </si>
+  <si>
+    <t>Chiefs</t>
+  </si>
+  <si>
+    <t>Panthers</t>
+  </si>
+  <si>
+    <t>Cardinals</t>
+  </si>
+  <si>
+    <t>Buccaneers</t>
+  </si>
+  <si>
+    <t>Raiders</t>
+  </si>
+  <si>
+    <t>Saints</t>
+  </si>
+  <si>
+    <t>Seahawks</t>
+  </si>
+  <si>
+    <t>Texans</t>
+  </si>
+  <si>
+    <t>Lions</t>
+  </si>
+  <si>
+    <t>Bills</t>
+  </si>
+  <si>
+    <t>Patriots</t>
+  </si>
+  <si>
+    <t>Browns</t>
+  </si>
+  <si>
+    <t>Jets</t>
+  </si>
+  <si>
+    <t>Broncos</t>
+  </si>
+  <si>
+    <t>Chargers</t>
+  </si>
+  <si>
+    <t>Falcons</t>
+  </si>
+  <si>
     <t>Packers</t>
   </si>
   <si>
+    <t>Cowboys</t>
+  </si>
+  <si>
+    <t>Eagles</t>
+  </si>
+  <si>
     <t>Bears</t>
   </si>
   <si>
-    <t xml:space="preserve"> </t>
-  </si>
-  <si>
-    <t>Rams</t>
-  </si>
-  <si>
-    <t>Giants</t>
-  </si>
-  <si>
-    <t>Chiefs</t>
-  </si>
-  <si>
-    <t>Saints</t>
-  </si>
-  <si>
-    <t>Titans</t>
-  </si>
-  <si>
-    <t>Colts</t>
-  </si>
-  <si>
-    <t>Eagles</t>
-  </si>
-  <si>
     <t>Vikings</t>
-  </si>
-  <si>
-    <t>Browns</t>
-  </si>
-  <si>
-    <t>Bengals</t>
-  </si>
-  <si>
-    <t>Lions</t>
-  </si>
-  <si>
-    <t>Washington</t>
-  </si>
-  <si>
-    <t>Jaguars</t>
-  </si>
-  <si>
-    <t>Raiders</t>
-  </si>
-  <si>
-    <t>Dolphins</t>
-  </si>
-  <si>
-    <t>Bills</t>
-  </si>
-  <si>
-    <t>Jets</t>
-  </si>
-  <si>
-    <t>Ravens</t>
-  </si>
-  <si>
-    <t>49ers</t>
-  </si>
-  <si>
-    <t>Buccaneers</t>
-  </si>
-  <si>
-    <t>Falcons</t>
-  </si>
-  <si>
-    <t>Chargers</t>
-  </si>
-  <si>
-    <t>Steelers</t>
-  </si>
-  <si>
-    <t>Patriots</t>
-  </si>
-  <si>
-    <t>Cardinals</t>
-  </si>
-  <si>
-    <t>Seahawks</t>
-  </si>
-  <si>
-    <t>Broncos</t>
-  </si>
-  <si>
-    <t>Texans</t>
   </si>
 </sst>
 </file>
@@ -186,10 +174,42 @@
     <numFmt numFmtId="165" formatCode="#0.0"/>
     <numFmt numFmtId="166" formatCode="#0"/>
   </numFmts>
-  <fonts count="24">
+  <fonts count="19">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF0D254C"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFD7A22A"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -205,31 +225,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFDD4814"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFC9AF74"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFCA001A"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -245,7 +241,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF000000"/>
+      <color rgb="FF69BE28"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -253,7 +249,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF0D254C"/>
+      <color rgb="FFB31B34"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -261,7 +257,47 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color rgb="FFC5C7CA"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFC60C30"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFC80819"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFE3C00"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF002244"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFB81C"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -277,7 +313,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFF0BF00"/>
+      <color rgb="FFDD4814"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -285,101 +321,13 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFE3C00"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFC5C7CA"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFD7A22A"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFF58120"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFC60C30"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFD0B240"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFE6BE8A"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFB81C"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFC80819"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF69BE28"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF002244"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFB31B34"/>
+      <color rgb="FFF0BF00"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="31">
+  <fills count="27">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -388,25 +336,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF203731"/>
+        <fgColor rgb="FF648FCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF03202F"/>
+        <fgColor rgb="FF006576"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF13264B"/>
+        <fgColor rgb="FFFB4F14"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF192F6B"/>
+        <fgColor rgb="FF773141"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF003B7B"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -418,61 +372,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFD2B887"/>
+        <fgColor rgb="FF0067CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF648FCC"/>
+        <fgColor rgb="FF9B2743"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF003B7B"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF003B48"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF3B0160"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF26201E"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFB4F14"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF006DB0"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF773141"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF006576"/>
+        <fgColor rgb="FFD60A0B"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -484,67 +396,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF008D97"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF00338D"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF0C371D"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF280353"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFAF1E2C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFD60A0B"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFBD0D18"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF0072CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFB612"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF0D254C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF9B2743"/>
+        <fgColor rgb="FFD2B887"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -557,6 +409,78 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF02253A"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF006DB0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00338D"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF0D254C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF26201E"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF0C371D"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF0072CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFBD0D18"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF203731"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC5CED6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF003B48"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF03202F"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF3B0160"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -588,7 +512,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -620,76 +544,64 @@
     <xf numFmtId="0" fontId="7" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="15" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="15" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="16" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="16" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="17" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="17" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="18" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="18" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="19" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="19" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="20" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="21" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="20" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="22" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="21" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="23" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="22" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="24" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="23" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="25" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="24" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="26" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="25" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="27" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="28" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="29" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="30" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="26" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1015,10 +927,10 @@
         <v>0</v>
       </c>
       <c r="B2" s="4">
-        <v>0.700352359929528</v>
+        <v>0.626559274688145</v>
       </c>
       <c r="C2" s="4">
-        <v>0.299647640070472</v>
+        <v>0.373440725311855</v>
       </c>
     </row>
     <row r="3" spans="1:61">
@@ -1026,10 +938,10 @@
         <v>1</v>
       </c>
       <c r="B3" s="5">
-        <v>24.2018037596392</v>
+        <v>24.7115368576926</v>
       </c>
       <c r="C3" s="5">
-        <v>16.1220019755996</v>
+        <v>19.4532737093453</v>
       </c>
     </row>
     <row r="4" spans="1:61">
@@ -1051,7 +963,7 @@
         <v>10</v>
       </c>
       <c r="C5" s="6">
-        <v>3</v>
+        <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:61">
@@ -1062,7 +974,7 @@
         <v>13</v>
       </c>
       <c r="C6" s="6">
-        <v>6</v>
+        <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:61">
@@ -1070,10 +982,10 @@
         <v>5</v>
       </c>
       <c r="B7" s="6">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C7" s="6">
-        <v>7</v>
+        <v>10</v>
       </c>
     </row>
     <row r="8" spans="1:61">
@@ -1084,7 +996,7 @@
         <v>16</v>
       </c>
       <c r="C8" s="6">
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
     <row r="9" spans="1:61">
@@ -1095,7 +1007,7 @@
         <v>17</v>
       </c>
       <c r="C9" s="6">
-        <v>10</v>
+        <v>13</v>
       </c>
     </row>
     <row r="10" spans="1:61">
@@ -1106,7 +1018,7 @@
         <v>19</v>
       </c>
       <c r="C10" s="6">
-        <v>10</v>
+        <v>14</v>
       </c>
     </row>
     <row r="11" spans="1:61">
@@ -1117,7 +1029,7 @@
         <v>20</v>
       </c>
       <c r="C11" s="6">
-        <v>13</v>
+        <v>16</v>
       </c>
     </row>
     <row r="12" spans="1:61">
@@ -1128,7 +1040,7 @@
         <v>22</v>
       </c>
       <c r="C12" s="6">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="13" spans="1:61">
@@ -1136,10 +1048,10 @@
         <v>11</v>
       </c>
       <c r="B13" s="6">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C13" s="6">
-        <v>15</v>
+        <v>19</v>
       </c>
     </row>
     <row r="14" spans="1:61">
@@ -1147,10 +1059,10 @@
         <v>12</v>
       </c>
       <c r="B14" s="6">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C14" s="6">
-        <v>17</v>
+        <v>20</v>
       </c>
     </row>
     <row r="15" spans="1:61">
@@ -1158,10 +1070,10 @@
         <v>13</v>
       </c>
       <c r="B15" s="6">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C15" s="6">
-        <v>17</v>
+        <v>21</v>
       </c>
     </row>
     <row r="16" spans="1:61">
@@ -1169,10 +1081,10 @@
         <v>14</v>
       </c>
       <c r="B16" s="6">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C16" s="6">
-        <v>20</v>
+        <v>23</v>
       </c>
     </row>
     <row r="17" spans="1:3">
@@ -1183,7 +1095,7 @@
         <v>30</v>
       </c>
       <c r="C17" s="6">
-        <v>20</v>
+        <v>24</v>
       </c>
     </row>
     <row r="18" spans="1:3">
@@ -1191,10 +1103,10 @@
         <v>16</v>
       </c>
       <c r="B18" s="6">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C18" s="6">
-        <v>23</v>
+        <v>26</v>
       </c>
     </row>
     <row r="19" spans="1:3">
@@ -1202,10 +1114,10 @@
         <v>17</v>
       </c>
       <c r="B19" s="6">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C19" s="6">
-        <v>24</v>
+        <v>28</v>
       </c>
     </row>
     <row r="20" spans="1:3">
@@ -1216,7 +1128,7 @@
         <v>37</v>
       </c>
       <c r="C20" s="6">
-        <v>27</v>
+        <v>30</v>
       </c>
     </row>
     <row r="21" spans="1:3">
@@ -1224,10 +1136,10 @@
         <v>19</v>
       </c>
       <c r="B21" s="6">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C21" s="6">
-        <v>30</v>
+        <v>34</v>
       </c>
     </row>
     <row r="22" spans="1:3">
@@ -1235,10 +1147,10 @@
         <v>20</v>
       </c>
       <c r="B22" s="6">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="C22" s="6">
-        <v>34</v>
+        <v>38</v>
       </c>
     </row>
   </sheetData>
@@ -1277,10 +1189,10 @@
         <v>0</v>
       </c>
       <c r="B2" s="4">
-        <v>0.402704819459036</v>
+        <v>0.451347009730598</v>
       </c>
       <c r="C2" s="4">
-        <v>0.597295180540964</v>
+        <v>0.548652990269402</v>
       </c>
     </row>
     <row r="3" spans="1:61">
@@ -1288,10 +1200,10 @@
         <v>1</v>
       </c>
       <c r="B3" s="5">
-        <v>16.8797908240418</v>
+        <v>21.3759675248065</v>
       </c>
       <c r="C3" s="5">
-        <v>20.5166924966615</v>
+        <v>23.4118235176353</v>
       </c>
     </row>
     <row r="4" spans="1:61">
@@ -1299,10 +1211,10 @@
         <v>2</v>
       </c>
       <c r="B4" s="6">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="C4" s="6">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:61">
@@ -1310,10 +1222,10 @@
         <v>3</v>
       </c>
       <c r="B5" s="6">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C5" s="6">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:61">
@@ -1321,10 +1233,10 @@
         <v>4</v>
       </c>
       <c r="B6" s="6">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C6" s="6">
-        <v>9</v>
+        <v>12</v>
       </c>
     </row>
     <row r="7" spans="1:61">
@@ -1332,10 +1244,10 @@
         <v>5</v>
       </c>
       <c r="B7" s="6">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="C7" s="6">
-        <v>10</v>
+        <v>13</v>
       </c>
     </row>
     <row r="8" spans="1:61">
@@ -1343,10 +1255,10 @@
         <v>6</v>
       </c>
       <c r="B8" s="6">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="C8" s="6">
-        <v>13</v>
+        <v>15</v>
       </c>
     </row>
     <row r="9" spans="1:61">
@@ -1354,10 +1266,10 @@
         <v>7</v>
       </c>
       <c r="B9" s="6">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C9" s="6">
-        <v>14</v>
+        <v>16</v>
       </c>
     </row>
     <row r="10" spans="1:61">
@@ -1365,10 +1277,10 @@
         <v>8</v>
       </c>
       <c r="B10" s="6">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="C10" s="6">
-        <v>16</v>
+        <v>18</v>
       </c>
     </row>
     <row r="11" spans="1:61">
@@ -1376,10 +1288,10 @@
         <v>9</v>
       </c>
       <c r="B11" s="6">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="C11" s="6">
-        <v>17</v>
+        <v>20</v>
       </c>
     </row>
     <row r="12" spans="1:61">
@@ -1387,10 +1299,10 @@
         <v>10</v>
       </c>
       <c r="B12" s="6">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="C12" s="6">
-        <v>17</v>
+        <v>21</v>
       </c>
     </row>
     <row r="13" spans="1:61">
@@ -1398,10 +1310,10 @@
         <v>11</v>
       </c>
       <c r="B13" s="6">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="C13" s="6">
-        <v>20</v>
+        <v>23</v>
       </c>
     </row>
     <row r="14" spans="1:61">
@@ -1409,10 +1321,10 @@
         <v>12</v>
       </c>
       <c r="B14" s="6">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="C14" s="6">
-        <v>21</v>
+        <v>24</v>
       </c>
     </row>
     <row r="15" spans="1:61">
@@ -1420,10 +1332,10 @@
         <v>13</v>
       </c>
       <c r="B15" s="6">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="C15" s="6">
-        <v>23</v>
+        <v>26</v>
       </c>
     </row>
     <row r="16" spans="1:61">
@@ -1431,10 +1343,10 @@
         <v>14</v>
       </c>
       <c r="B16" s="6">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="C16" s="6">
-        <v>24</v>
+        <v>27</v>
       </c>
     </row>
     <row r="17" spans="1:3">
@@ -1442,10 +1354,10 @@
         <v>15</v>
       </c>
       <c r="B17" s="6">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="C17" s="6">
-        <v>26</v>
+        <v>29</v>
       </c>
     </row>
     <row r="18" spans="1:3">
@@ -1453,10 +1365,10 @@
         <v>16</v>
       </c>
       <c r="B18" s="6">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="C18" s="6">
-        <v>27</v>
+        <v>31</v>
       </c>
     </row>
     <row r="19" spans="1:3">
@@ -1464,10 +1376,10 @@
         <v>17</v>
       </c>
       <c r="B19" s="6">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="C19" s="6">
-        <v>30</v>
+        <v>33</v>
       </c>
     </row>
     <row r="20" spans="1:3">
@@ -1475,10 +1387,10 @@
         <v>18</v>
       </c>
       <c r="B20" s="6">
-        <v>26</v>
+        <v>33</v>
       </c>
       <c r="C20" s="6">
-        <v>32</v>
+        <v>36</v>
       </c>
     </row>
     <row r="21" spans="1:3">
@@ -1486,10 +1398,10 @@
         <v>19</v>
       </c>
       <c r="B21" s="6">
-        <v>29</v>
+        <v>37</v>
       </c>
       <c r="C21" s="6">
-        <v>36</v>
+        <v>39</v>
       </c>
     </row>
     <row r="22" spans="1:3">
@@ -1497,10 +1409,10 @@
         <v>20</v>
       </c>
       <c r="B22" s="6">
-        <v>33</v>
+        <v>41</v>
       </c>
       <c r="C22" s="6">
-        <v>41</v>
+        <v>44</v>
       </c>
     </row>
   </sheetData>
@@ -1510,7 +1422,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:BO22"/>
+  <dimension ref="A1:BI22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
@@ -1520,17 +1432,16 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="20.7109375" customWidth="1"/>
-    <col min="2" max="24" width="12.7109375" customWidth="1"/>
+    <col min="2" max="21" width="12.7109375" customWidth="1"/>
     <col min="4" max="4" width="0.85546875" customWidth="1"/>
     <col min="7" max="7" width="0.85546875" customWidth="1"/>
     <col min="10" max="10" width="0.85546875" customWidth="1"/>
     <col min="13" max="13" width="0.85546875" customWidth="1"/>
     <col min="16" max="16" width="0.85546875" customWidth="1"/>
     <col min="19" max="19" width="0.85546875" customWidth="1"/>
-    <col min="22" max="22" width="0.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:67">
+    <row r="1" spans="1:61">
       <c r="B1" s="9" t="s">
         <v>26</v>
       </c>
@@ -1576,15 +1487,6 @@
       <c r="U1" s="22" t="s">
         <v>39</v>
       </c>
-      <c r="V1" t="s">
-        <v>23</v>
-      </c>
-      <c r="W1" s="23" t="s">
-        <v>40</v>
-      </c>
-      <c r="X1" s="24" t="s">
-        <v>41</v>
-      </c>
       <c r="AE1" t="s">
         <v>23</v>
       </c>
@@ -1600,1121 +1502,992 @@
       <c r="BI1" t="s">
         <v>23</v>
       </c>
-      <c r="BO1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="2" spans="1:67">
+    </row>
+    <row r="2" spans="1:61">
       <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="4">
-        <v>0.547267390546522</v>
+        <v>0.446115210776958</v>
       </c>
       <c r="C2" s="4">
-        <v>0.452732609453478</v>
+        <v>0.553884789223042</v>
       </c>
       <c r="E2" s="4">
-        <v>0.5061109987778</v>
+        <v>0.277478444504311</v>
       </c>
       <c r="F2" s="4">
-        <v>0.4938890012222</v>
+        <v>0.722521555495689</v>
       </c>
       <c r="H2" s="4">
-        <v>0.50342359931528</v>
+        <v>0.373665025266995</v>
       </c>
       <c r="I2" s="4">
-        <v>0.49657640068472</v>
+        <v>0.626334974733005</v>
       </c>
       <c r="K2" s="4">
-        <v>0.346136730772654</v>
+        <v>0.391591421681716</v>
       </c>
       <c r="L2" s="4">
-        <v>0.653863269227346</v>
+        <v>0.608408578318284</v>
       </c>
       <c r="N2" s="4">
-        <v>0.49062710187458</v>
+        <v>0.50060729987854</v>
       </c>
       <c r="O2" s="4">
-        <v>0.50937289812542</v>
+        <v>0.49939270012146</v>
       </c>
       <c r="Q2" s="4">
-        <v>0.407359218528156</v>
+        <v>0.4999165000167</v>
       </c>
       <c r="R2" s="4">
-        <v>0.592640781471844</v>
+        <v>0.5000834999833</v>
       </c>
       <c r="T2" s="4">
-        <v>0.225882854823429</v>
+        <v>0.415691416861717</v>
       </c>
       <c r="U2" s="4">
-        <v>0.774117145176571</v>
-      </c>
-      <c r="W2" s="4">
-        <v>0.285878542824291</v>
-      </c>
-      <c r="X2" s="4">
-        <v>0.714121457175709</v>
-      </c>
-    </row>
-    <row r="3" spans="1:67">
+        <v>0.584308583138283</v>
+      </c>
+    </row>
+    <row r="3" spans="1:61">
       <c r="A3" s="3" t="s">
         <v>1</v>
       </c>
       <c r="B3" s="5">
-        <v>28.7466870506626</v>
+        <v>24.7203606559279</v>
       </c>
       <c r="C3" s="5">
-        <v>26.4676829064634</v>
+        <v>27.1044265791147</v>
       </c>
       <c r="E3" s="5">
-        <v>25.7533884493223</v>
+        <v>18.4223125155375</v>
       </c>
       <c r="F3" s="5">
-        <v>25.4256621148676</v>
+        <v>28.425169914966</v>
       </c>
       <c r="H3" s="5">
-        <v>16.6784132643173</v>
+        <v>22.7368458526308</v>
       </c>
       <c r="I3" s="5">
-        <v>16.5867530826494</v>
+        <v>28.5786364842727</v>
       </c>
       <c r="K3" s="5">
-        <v>20.7910834417833</v>
+        <v>19.803529839294</v>
       </c>
       <c r="L3" s="5">
-        <v>27.4778559044288</v>
+        <v>24.3917647216471</v>
       </c>
       <c r="N3" s="5">
-        <v>26.0757113848577</v>
+        <v>21.4241269151746</v>
       </c>
       <c r="O3" s="5">
-        <v>26.4914787017043</v>
+        <v>21.3999611200078</v>
       </c>
       <c r="Q3" s="5">
-        <v>22.6596728680654</v>
+        <v>20.6485816702837</v>
       </c>
       <c r="R3" s="5">
-        <v>26.8163242367352</v>
+        <v>20.6426670714666</v>
       </c>
       <c r="T3" s="5">
-        <v>15.7067438586512</v>
+        <v>23.4809293038141</v>
       </c>
       <c r="U3" s="5">
-        <v>27.6978728604254</v>
-      </c>
-      <c r="W3" s="5">
-        <v>14.4299233140153</v>
-      </c>
-      <c r="X3" s="5">
-        <v>22.9182120163576</v>
-      </c>
-    </row>
-    <row r="4" spans="1:67">
+        <v>27.2487111502578</v>
+      </c>
+    </row>
+    <row r="4" spans="1:61">
       <c r="A4" s="3" t="s">
         <v>2</v>
       </c>
       <c r="B4" s="6">
+        <v>7</v>
+      </c>
+      <c r="C4" s="6">
         <v>9</v>
       </c>
-      <c r="C4" s="6">
+      <c r="E4" s="6">
+        <v>3</v>
+      </c>
+      <c r="F4" s="6">
+        <v>9</v>
+      </c>
+      <c r="H4" s="6">
+        <v>6</v>
+      </c>
+      <c r="I4" s="6">
+        <v>8</v>
+      </c>
+      <c r="K4" s="6">
+        <v>3</v>
+      </c>
+      <c r="L4" s="6">
         <v>7</v>
       </c>
-      <c r="E4" s="6">
-        <v>7</v>
-      </c>
-      <c r="F4" s="6">
+      <c r="N4" s="6">
+        <v>6</v>
+      </c>
+      <c r="O4" s="6">
+        <v>6</v>
+      </c>
+      <c r="Q4" s="6">
+        <v>3</v>
+      </c>
+      <c r="R4" s="6">
+        <v>4</v>
+      </c>
+      <c r="T4" s="6">
+        <v>6</v>
+      </c>
+      <c r="U4" s="6">
         <v>8</v>
       </c>
-      <c r="H4" s="6">
-        <v>3</v>
-      </c>
-      <c r="I4" s="6">
-        <v>0</v>
-      </c>
-      <c r="K4" s="6">
-        <v>5</v>
-      </c>
-      <c r="L4" s="6">
-        <v>9</v>
-      </c>
-      <c r="N4" s="6">
-        <v>7</v>
-      </c>
-      <c r="O4" s="6">
-        <v>9</v>
-      </c>
-      <c r="Q4" s="6">
-        <v>6</v>
-      </c>
-      <c r="R4" s="6">
-        <v>7</v>
-      </c>
-      <c r="T4" s="6">
-        <v>3</v>
-      </c>
-      <c r="U4" s="6">
-        <v>9</v>
-      </c>
-      <c r="W4" s="6">
-        <v>0</v>
-      </c>
-      <c r="X4" s="6">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="5" spans="1:67">
+    </row>
+    <row r="5" spans="1:61">
       <c r="A5" s="3" t="s">
         <v>3</v>
       </c>
       <c r="B5" s="6">
+        <v>10</v>
+      </c>
+      <c r="C5" s="6">
+        <v>12</v>
+      </c>
+      <c r="E5" s="6">
+        <v>6</v>
+      </c>
+      <c r="F5" s="6">
         <v>13</v>
       </c>
-      <c r="C5" s="6">
-        <v>10</v>
-      </c>
-      <c r="E5" s="6">
-        <v>10</v>
-      </c>
-      <c r="F5" s="6">
-        <v>10</v>
-      </c>
       <c r="H5" s="6">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="I5" s="6">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="K5" s="6">
         <v>7</v>
       </c>
       <c r="L5" s="6">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="N5" s="6">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="O5" s="6">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="Q5" s="6">
         <v>7</v>
       </c>
       <c r="R5" s="6">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="T5" s="6">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="U5" s="6">
         <v>12</v>
       </c>
-      <c r="W5" s="6">
-        <v>3</v>
-      </c>
-      <c r="X5" s="6">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="6" spans="1:67">
+    </row>
+    <row r="6" spans="1:61">
       <c r="A6" s="3" t="s">
         <v>4</v>
       </c>
       <c r="B6" s="6">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C6" s="6">
         <v>14</v>
       </c>
       <c r="E6" s="6">
+        <v>7</v>
+      </c>
+      <c r="F6" s="6">
+        <v>15</v>
+      </c>
+      <c r="H6" s="6">
+        <v>10</v>
+      </c>
+      <c r="I6" s="6">
+        <v>14</v>
+      </c>
+      <c r="K6" s="6">
+        <v>7</v>
+      </c>
+      <c r="L6" s="6">
         <v>13</v>
       </c>
-      <c r="F6" s="6">
-        <v>13</v>
-      </c>
-      <c r="H6" s="6">
-        <v>7</v>
-      </c>
-      <c r="I6" s="6">
-        <v>7</v>
-      </c>
-      <c r="K6" s="6">
+      <c r="N6" s="6">
+        <v>10</v>
+      </c>
+      <c r="O6" s="6">
+        <v>10</v>
+      </c>
+      <c r="Q6" s="6">
         <v>9</v>
       </c>
-      <c r="L6" s="6">
-        <v>14</v>
-      </c>
-      <c r="N6" s="6">
-        <v>13</v>
-      </c>
-      <c r="O6" s="6">
-        <v>13</v>
-      </c>
-      <c r="Q6" s="6">
+      <c r="R6" s="6">
+        <v>9</v>
+      </c>
+      <c r="T6" s="6">
         <v>10</v>
-      </c>
-      <c r="R6" s="6">
-        <v>13</v>
-      </c>
-      <c r="T6" s="6">
-        <v>6</v>
       </c>
       <c r="U6" s="6">
         <v>14</v>
       </c>
-      <c r="W6" s="6">
-        <v>6</v>
-      </c>
-      <c r="X6" s="6">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="7" spans="1:67">
+    </row>
+    <row r="7" spans="1:61">
       <c r="A7" s="3" t="s">
         <v>5</v>
       </c>
       <c r="B7" s="6">
+        <v>14</v>
+      </c>
+      <c r="C7" s="6">
+        <v>16</v>
+      </c>
+      <c r="E7" s="6">
+        <v>9</v>
+      </c>
+      <c r="F7" s="6">
         <v>17</v>
       </c>
-      <c r="C7" s="6">
+      <c r="H7" s="6">
+        <v>13</v>
+      </c>
+      <c r="I7" s="6">
+        <v>17</v>
+      </c>
+      <c r="K7" s="6">
+        <v>10</v>
+      </c>
+      <c r="L7" s="6">
         <v>14</v>
       </c>
-      <c r="E7" s="6">
-        <v>15</v>
-      </c>
-      <c r="F7" s="6">
-        <v>16</v>
-      </c>
-      <c r="H7" s="6">
-        <v>8</v>
-      </c>
-      <c r="I7" s="6">
-        <v>7</v>
-      </c>
-      <c r="K7" s="6">
-        <v>11</v>
-      </c>
-      <c r="L7" s="6">
-        <v>17</v>
-      </c>
       <c r="N7" s="6">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="O7" s="6">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="Q7" s="6">
+        <v>10</v>
+      </c>
+      <c r="R7" s="6">
+        <v>10</v>
+      </c>
+      <c r="T7" s="6">
         <v>13</v>
-      </c>
-      <c r="R7" s="6">
-        <v>16</v>
-      </c>
-      <c r="T7" s="6">
-        <v>7</v>
       </c>
       <c r="U7" s="6">
         <v>16</v>
       </c>
-      <c r="W7" s="6">
-        <v>7</v>
-      </c>
-      <c r="X7" s="6">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="8" spans="1:67">
+    </row>
+    <row r="8" spans="1:61">
       <c r="A8" s="3" t="s">
         <v>6</v>
       </c>
       <c r="B8" s="6">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="C8" s="6">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E8" s="6">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="F8" s="6">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="H8" s="6">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="I8" s="6">
-        <v>9</v>
+        <v>19</v>
       </c>
       <c r="K8" s="6">
+        <v>11</v>
+      </c>
+      <c r="L8" s="6">
+        <v>16</v>
+      </c>
+      <c r="N8" s="6">
         <v>13</v>
       </c>
-      <c r="L8" s="6">
+      <c r="O8" s="6">
+        <v>13</v>
+      </c>
+      <c r="Q8" s="6">
+        <v>13</v>
+      </c>
+      <c r="R8" s="6">
+        <v>13</v>
+      </c>
+      <c r="T8" s="6">
+        <v>14</v>
+      </c>
+      <c r="U8" s="6">
         <v>18</v>
       </c>
-      <c r="N8" s="6">
-        <v>17</v>
-      </c>
-      <c r="O8" s="6">
-        <v>17</v>
-      </c>
-      <c r="Q8" s="6">
-        <v>14</v>
-      </c>
-      <c r="R8" s="6">
-        <v>17</v>
-      </c>
-      <c r="T8" s="6">
-        <v>9</v>
-      </c>
-      <c r="U8" s="6">
-        <v>19</v>
-      </c>
-      <c r="W8" s="6">
-        <v>7</v>
-      </c>
-      <c r="X8" s="6">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="9" spans="1:67">
+    </row>
+    <row r="9" spans="1:61">
       <c r="A9" s="3" t="s">
         <v>7</v>
       </c>
       <c r="B9" s="6">
+        <v>17</v>
+      </c>
+      <c r="C9" s="6">
+        <v>20</v>
+      </c>
+      <c r="E9" s="6">
+        <v>13</v>
+      </c>
+      <c r="F9" s="6">
         <v>21</v>
       </c>
-      <c r="C9" s="6">
-        <v>19</v>
-      </c>
-      <c r="E9" s="6">
-        <v>19</v>
-      </c>
-      <c r="F9" s="6">
-        <v>19</v>
-      </c>
       <c r="H9" s="6">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="I9" s="6">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="K9" s="6">
         <v>14</v>
       </c>
       <c r="L9" s="6">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="N9" s="6">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="O9" s="6">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="Q9" s="6">
+        <v>14</v>
+      </c>
+      <c r="R9" s="6">
+        <v>14</v>
+      </c>
+      <c r="T9" s="6">
         <v>16</v>
-      </c>
-      <c r="R9" s="6">
-        <v>20</v>
-      </c>
-      <c r="T9" s="6">
-        <v>10</v>
       </c>
       <c r="U9" s="6">
         <v>20</v>
       </c>
-      <c r="W9" s="6">
-        <v>9</v>
-      </c>
-      <c r="X9" s="6">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="10" spans="1:67">
+    </row>
+    <row r="10" spans="1:61">
       <c r="A10" s="3" t="s">
         <v>8</v>
       </c>
       <c r="B10" s="6">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C10" s="6">
         <v>21</v>
       </c>
       <c r="E10" s="6">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="F10" s="6">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="H10" s="6">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="I10" s="6">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="K10" s="6">
+        <v>14</v>
+      </c>
+      <c r="L10" s="6">
+        <v>19</v>
+      </c>
+      <c r="N10" s="6">
         <v>16</v>
       </c>
-      <c r="L10" s="6">
-        <v>22</v>
-      </c>
-      <c r="N10" s="6">
-        <v>20</v>
-      </c>
       <c r="O10" s="6">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="Q10" s="6">
+        <v>14</v>
+      </c>
+      <c r="R10" s="6">
+        <v>16</v>
+      </c>
+      <c r="T10" s="6">
         <v>17</v>
       </c>
-      <c r="R10" s="6">
+      <c r="U10" s="6">
         <v>21</v>
       </c>
-      <c r="T10" s="6">
-        <v>10</v>
-      </c>
-      <c r="U10" s="6">
-        <v>22</v>
-      </c>
-      <c r="W10" s="6">
-        <v>10</v>
-      </c>
-      <c r="X10" s="6">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="11" spans="1:67">
+    </row>
+    <row r="11" spans="1:61">
       <c r="A11" s="3" t="s">
         <v>9</v>
       </c>
       <c r="B11" s="6">
+        <v>20</v>
+      </c>
+      <c r="C11" s="6">
+        <v>23</v>
+      </c>
+      <c r="E11" s="6">
+        <v>14</v>
+      </c>
+      <c r="F11" s="6">
         <v>24</v>
       </c>
-      <c r="C11" s="6">
-        <v>21</v>
-      </c>
-      <c r="E11" s="6">
-        <v>22</v>
-      </c>
-      <c r="F11" s="6">
-        <v>22</v>
-      </c>
       <c r="H11" s="6">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="I11" s="6">
-        <v>13</v>
+        <v>24</v>
       </c>
       <c r="K11" s="6">
+        <v>16</v>
+      </c>
+      <c r="L11" s="6">
+        <v>20</v>
+      </c>
+      <c r="N11" s="6">
         <v>17</v>
       </c>
-      <c r="L11" s="6">
-        <v>23</v>
-      </c>
-      <c r="N11" s="6">
-        <v>22</v>
-      </c>
       <c r="O11" s="6">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="Q11" s="6">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="R11" s="6">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="T11" s="6">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="U11" s="6">
         <v>23</v>
       </c>
-      <c r="W11" s="6">
-        <v>10</v>
-      </c>
-      <c r="X11" s="6">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="12" spans="1:67">
+    </row>
+    <row r="12" spans="1:61">
       <c r="A12" s="3" t="s">
         <v>10</v>
       </c>
       <c r="B12" s="6">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="C12" s="6">
         <v>24</v>
       </c>
       <c r="E12" s="6">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="F12" s="6">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="H12" s="6">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="I12" s="6">
-        <v>14</v>
+        <v>26</v>
       </c>
       <c r="K12" s="6">
+        <v>17</v>
+      </c>
+      <c r="L12" s="6">
+        <v>22</v>
+      </c>
+      <c r="N12" s="6">
         <v>19</v>
       </c>
-      <c r="L12" s="6">
-        <v>25</v>
-      </c>
-      <c r="N12" s="6">
+      <c r="O12" s="6">
+        <v>19</v>
+      </c>
+      <c r="Q12" s="6">
+        <v>17</v>
+      </c>
+      <c r="R12" s="6">
+        <v>18</v>
+      </c>
+      <c r="T12" s="6">
+        <v>21</v>
+      </c>
+      <c r="U12" s="6">
         <v>24</v>
       </c>
-      <c r="O12" s="6">
-        <v>24</v>
-      </c>
-      <c r="Q12" s="6">
-        <v>20</v>
-      </c>
-      <c r="R12" s="6">
-        <v>24</v>
-      </c>
-      <c r="T12" s="6">
-        <v>13</v>
-      </c>
-      <c r="U12" s="6">
-        <v>25</v>
-      </c>
-      <c r="W12" s="6">
-        <v>13</v>
-      </c>
-      <c r="X12" s="6">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="13" spans="1:67">
+    </row>
+    <row r="13" spans="1:61">
       <c r="A13" s="3" t="s">
         <v>11</v>
       </c>
       <c r="B13" s="6">
+        <v>24</v>
+      </c>
+      <c r="C13" s="6">
+        <v>26</v>
+      </c>
+      <c r="E13" s="6">
+        <v>17</v>
+      </c>
+      <c r="F13" s="6">
         <v>27</v>
       </c>
-      <c r="C13" s="6">
-        <v>25</v>
-      </c>
-      <c r="E13" s="6">
-        <v>25</v>
-      </c>
-      <c r="F13" s="6">
-        <v>24</v>
-      </c>
       <c r="H13" s="6">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="I13" s="6">
-        <v>15</v>
+        <v>27</v>
       </c>
       <c r="K13" s="6">
+        <v>19</v>
+      </c>
+      <c r="L13" s="6">
+        <v>23</v>
+      </c>
+      <c r="N13" s="6">
         <v>20</v>
       </c>
-      <c r="L13" s="6">
+      <c r="O13" s="6">
+        <v>20</v>
+      </c>
+      <c r="Q13" s="6">
+        <v>20</v>
+      </c>
+      <c r="R13" s="6">
+        <v>20</v>
+      </c>
+      <c r="T13" s="6">
+        <v>23</v>
+      </c>
+      <c r="U13" s="6">
         <v>26</v>
       </c>
-      <c r="N13" s="6">
-        <v>24</v>
-      </c>
-      <c r="O13" s="6">
-        <v>26</v>
-      </c>
-      <c r="Q13" s="6">
-        <v>21</v>
-      </c>
-      <c r="R13" s="6">
-        <v>26</v>
-      </c>
-      <c r="T13" s="6">
-        <v>14</v>
-      </c>
-      <c r="U13" s="6">
-        <v>27</v>
-      </c>
-      <c r="W13" s="6">
-        <v>13</v>
-      </c>
-      <c r="X13" s="6">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="14" spans="1:67">
+    </row>
+    <row r="14" spans="1:61">
       <c r="A14" s="3" t="s">
         <v>12</v>
       </c>
       <c r="B14" s="6">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="C14" s="6">
         <v>27</v>
       </c>
       <c r="E14" s="6">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="F14" s="6">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="H14" s="6">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="I14" s="6">
-        <v>17</v>
+        <v>29</v>
       </c>
       <c r="K14" s="6">
         <v>21</v>
       </c>
       <c r="L14" s="6">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="N14" s="6">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="O14" s="6">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="Q14" s="6">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="R14" s="6">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="T14" s="6">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="U14" s="6">
         <v>28</v>
       </c>
-      <c r="W14" s="6">
-        <v>14</v>
-      </c>
-      <c r="X14" s="6">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="15" spans="1:67">
+    </row>
+    <row r="15" spans="1:61">
       <c r="A15" s="3" t="s">
         <v>13</v>
       </c>
       <c r="B15" s="6">
+        <v>27</v>
+      </c>
+      <c r="C15" s="6">
+        <v>29</v>
+      </c>
+      <c r="E15" s="6">
+        <v>20</v>
+      </c>
+      <c r="F15" s="6">
         <v>31</v>
       </c>
-      <c r="C15" s="6">
-        <v>28</v>
-      </c>
-      <c r="E15" s="6">
-        <v>28</v>
-      </c>
-      <c r="F15" s="6">
-        <v>27</v>
-      </c>
       <c r="H15" s="6">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="I15" s="6">
-        <v>18</v>
+        <v>31</v>
       </c>
       <c r="K15" s="6">
+        <v>21</v>
+      </c>
+      <c r="L15" s="6">
+        <v>26</v>
+      </c>
+      <c r="N15" s="6">
         <v>23</v>
       </c>
-      <c r="L15" s="6">
-        <v>30</v>
-      </c>
-      <c r="N15" s="6">
-        <v>28</v>
-      </c>
       <c r="O15" s="6">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="Q15" s="6">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="R15" s="6">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="T15" s="6">
-        <v>17</v>
+        <v>26</v>
       </c>
       <c r="U15" s="6">
         <v>30</v>
       </c>
-      <c r="W15" s="6">
-        <v>16</v>
-      </c>
-      <c r="X15" s="6">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="16" spans="1:67">
+    </row>
+    <row r="16" spans="1:61">
       <c r="A16" s="3" t="s">
         <v>14</v>
       </c>
       <c r="B16" s="6">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="C16" s="6">
         <v>31</v>
       </c>
       <c r="E16" s="6">
-        <v>30</v>
+        <v>21</v>
       </c>
       <c r="F16" s="6">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="H16" s="6">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="I16" s="6">
-        <v>20</v>
+        <v>33</v>
       </c>
       <c r="K16" s="6">
         <v>24</v>
       </c>
       <c r="L16" s="6">
+        <v>28</v>
+      </c>
+      <c r="N16" s="6">
+        <v>24</v>
+      </c>
+      <c r="O16" s="6">
+        <v>24</v>
+      </c>
+      <c r="Q16" s="6">
+        <v>24</v>
+      </c>
+      <c r="R16" s="6">
+        <v>24</v>
+      </c>
+      <c r="T16" s="6">
+        <v>27</v>
+      </c>
+      <c r="U16" s="6">
         <v>31</v>
       </c>
-      <c r="N16" s="6">
-        <v>30</v>
-      </c>
-      <c r="O16" s="6">
-        <v>30</v>
-      </c>
-      <c r="Q16" s="6">
-        <v>27</v>
-      </c>
-      <c r="R16" s="6">
-        <v>31</v>
-      </c>
-      <c r="T16" s="6">
-        <v>19</v>
-      </c>
-      <c r="U16" s="6">
-        <v>32</v>
-      </c>
-      <c r="W16" s="6">
-        <v>17</v>
-      </c>
-      <c r="X16" s="6">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="17" spans="1:24">
+    </row>
+    <row r="17" spans="1:21">
       <c r="A17" s="3" t="s">
         <v>15</v>
       </c>
       <c r="B17" s="6">
+        <v>30</v>
+      </c>
+      <c r="C17" s="6">
+        <v>33</v>
+      </c>
+      <c r="E17" s="6">
+        <v>23</v>
+      </c>
+      <c r="F17" s="6">
+        <v>34</v>
+      </c>
+      <c r="H17" s="6">
+        <v>28</v>
+      </c>
+      <c r="I17" s="6">
         <v>35</v>
       </c>
-      <c r="C17" s="6">
-        <v>32</v>
-      </c>
-      <c r="E17" s="6">
-        <v>31</v>
-      </c>
-      <c r="F17" s="6">
-        <v>31</v>
-      </c>
-      <c r="H17" s="6">
-        <v>21</v>
-      </c>
-      <c r="I17" s="6">
-        <v>21</v>
-      </c>
       <c r="K17" s="6">
+        <v>24</v>
+      </c>
+      <c r="L17" s="6">
+        <v>30</v>
+      </c>
+      <c r="N17" s="6">
+        <v>27</v>
+      </c>
+      <c r="O17" s="6">
+        <v>27</v>
+      </c>
+      <c r="Q17" s="6">
         <v>26</v>
       </c>
-      <c r="L17" s="6">
+      <c r="R17" s="6">
+        <v>26</v>
+      </c>
+      <c r="T17" s="6">
+        <v>29</v>
+      </c>
+      <c r="U17" s="6">
         <v>33</v>
       </c>
-      <c r="N17" s="6">
-        <v>32</v>
-      </c>
-      <c r="O17" s="6">
-        <v>33</v>
-      </c>
-      <c r="Q17" s="6">
-        <v>28</v>
-      </c>
-      <c r="R17" s="6">
-        <v>33</v>
-      </c>
-      <c r="T17" s="6">
-        <v>20</v>
-      </c>
-      <c r="U17" s="6">
-        <v>34</v>
-      </c>
-      <c r="W17" s="6">
-        <v>19</v>
-      </c>
-      <c r="X17" s="6">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="18" spans="1:24">
+    </row>
+    <row r="18" spans="1:21">
       <c r="A18" s="3" t="s">
         <v>16</v>
       </c>
       <c r="B18" s="6">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="C18" s="6">
         <v>35</v>
       </c>
       <c r="E18" s="6">
-        <v>34</v>
+        <v>25</v>
       </c>
       <c r="F18" s="6">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="H18" s="6">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="I18" s="6">
-        <v>23</v>
+        <v>37</v>
       </c>
       <c r="K18" s="6">
+        <v>27</v>
+      </c>
+      <c r="L18" s="6">
+        <v>32</v>
+      </c>
+      <c r="N18" s="6">
         <v>28</v>
       </c>
-      <c r="L18" s="6">
+      <c r="O18" s="6">
+        <v>28</v>
+      </c>
+      <c r="Q18" s="6">
+        <v>28</v>
+      </c>
+      <c r="R18" s="6">
+        <v>27</v>
+      </c>
+      <c r="T18" s="6">
+        <v>31</v>
+      </c>
+      <c r="U18" s="6">
         <v>35</v>
       </c>
-      <c r="N18" s="6">
-        <v>34</v>
-      </c>
-      <c r="O18" s="6">
-        <v>34</v>
-      </c>
-      <c r="Q18" s="6">
-        <v>30</v>
-      </c>
-      <c r="R18" s="6">
-        <v>35</v>
-      </c>
-      <c r="T18" s="6">
-        <v>21</v>
-      </c>
-      <c r="U18" s="6">
-        <v>36</v>
-      </c>
-      <c r="W18" s="6">
-        <v>20</v>
-      </c>
-      <c r="X18" s="6">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="19" spans="1:24">
+    </row>
+    <row r="19" spans="1:21">
       <c r="A19" s="3" t="s">
         <v>17</v>
       </c>
       <c r="B19" s="6">
+        <v>34</v>
+      </c>
+      <c r="C19" s="6">
+        <v>37</v>
+      </c>
+      <c r="E19" s="6">
+        <v>27</v>
+      </c>
+      <c r="F19" s="6">
+        <v>39</v>
+      </c>
+      <c r="H19" s="6">
+        <v>33</v>
+      </c>
+      <c r="I19" s="6">
         <v>40</v>
       </c>
-      <c r="C19" s="6">
-        <v>38</v>
-      </c>
-      <c r="E19" s="6">
-        <v>36</v>
-      </c>
-      <c r="F19" s="6">
-        <v>35</v>
-      </c>
-      <c r="H19" s="6">
-        <v>24</v>
-      </c>
-      <c r="I19" s="6">
-        <v>24</v>
-      </c>
       <c r="K19" s="6">
+        <v>28</v>
+      </c>
+      <c r="L19" s="6">
+        <v>34</v>
+      </c>
+      <c r="N19" s="6">
         <v>30</v>
       </c>
-      <c r="L19" s="6">
-        <v>38</v>
-      </c>
-      <c r="N19" s="6">
-        <v>37</v>
-      </c>
       <c r="O19" s="6">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="Q19" s="6">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="R19" s="6">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="T19" s="6">
-        <v>23</v>
+        <v>34</v>
       </c>
       <c r="U19" s="6">
         <v>38</v>
       </c>
-      <c r="W19" s="6">
-        <v>22</v>
-      </c>
-      <c r="X19" s="6">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="20" spans="1:24">
+    </row>
+    <row r="20" spans="1:21">
       <c r="A20" s="3" t="s">
         <v>18</v>
       </c>
       <c r="B20" s="6">
+        <v>37</v>
+      </c>
+      <c r="C20" s="6">
+        <v>40</v>
+      </c>
+      <c r="E20" s="6">
+        <v>30</v>
+      </c>
+      <c r="F20" s="6">
+        <v>42</v>
+      </c>
+      <c r="H20" s="6">
+        <v>35</v>
+      </c>
+      <c r="I20" s="6">
         <v>43</v>
       </c>
-      <c r="C20" s="6">
-        <v>41</v>
-      </c>
-      <c r="E20" s="6">
-        <v>39</v>
-      </c>
-      <c r="F20" s="6">
-        <v>38</v>
-      </c>
-      <c r="H20" s="6">
-        <v>27</v>
-      </c>
-      <c r="I20" s="6">
-        <v>27</v>
-      </c>
       <c r="K20" s="6">
+        <v>31</v>
+      </c>
+      <c r="L20" s="6">
+        <v>37</v>
+      </c>
+      <c r="N20" s="6">
         <v>33</v>
       </c>
-      <c r="L20" s="6">
-        <v>41</v>
-      </c>
-      <c r="N20" s="6">
-        <v>39</v>
-      </c>
       <c r="O20" s="6">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="Q20" s="6">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="R20" s="6">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="T20" s="6">
-        <v>26</v>
+        <v>36</v>
       </c>
       <c r="U20" s="6">
         <v>41</v>
       </c>
-      <c r="W20" s="6">
-        <v>24</v>
-      </c>
-      <c r="X20" s="6">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="21" spans="1:24">
+    </row>
+    <row r="21" spans="1:21">
       <c r="A21" s="3" t="s">
         <v>19</v>
       </c>
       <c r="B21" s="6">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="C21" s="6">
         <v>44</v>
       </c>
       <c r="E21" s="6">
-        <v>43</v>
+        <v>33</v>
       </c>
       <c r="F21" s="6">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="H21" s="6">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="I21" s="6">
-        <v>30</v>
+        <v>47</v>
       </c>
       <c r="K21" s="6">
+        <v>35</v>
+      </c>
+      <c r="L21" s="6">
+        <v>40</v>
+      </c>
+      <c r="N21" s="6">
+        <v>37</v>
+      </c>
+      <c r="O21" s="6">
         <v>36</v>
       </c>
-      <c r="L21" s="6">
+      <c r="Q21" s="6">
+        <v>36</v>
+      </c>
+      <c r="R21" s="6">
+        <v>35</v>
+      </c>
+      <c r="T21" s="6">
+        <v>40</v>
+      </c>
+      <c r="U21" s="6">
         <v>44</v>
       </c>
-      <c r="N21" s="6">
-        <v>43</v>
-      </c>
-      <c r="O21" s="6">
-        <v>43</v>
-      </c>
-      <c r="Q21" s="6">
-        <v>38</v>
-      </c>
-      <c r="R21" s="6">
-        <v>44</v>
-      </c>
-      <c r="T21" s="6">
-        <v>28</v>
-      </c>
-      <c r="U21" s="6">
-        <v>45</v>
-      </c>
-      <c r="W21" s="6">
-        <v>27</v>
-      </c>
-      <c r="X21" s="6">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="22" spans="1:24">
+    </row>
+    <row r="22" spans="1:21">
       <c r="A22" s="3" t="s">
         <v>20</v>
       </c>
       <c r="B22" s="6">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="C22" s="6">
         <v>50</v>
       </c>
       <c r="E22" s="6">
-        <v>48</v>
+        <v>37</v>
       </c>
       <c r="F22" s="6">
-        <v>47</v>
+        <v>52</v>
       </c>
       <c r="H22" s="6">
-        <v>34</v>
+        <v>44</v>
       </c>
       <c r="I22" s="6">
-        <v>35</v>
+        <v>53</v>
       </c>
       <c r="K22" s="6">
         <v>41</v>
       </c>
       <c r="L22" s="6">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="N22" s="6">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="O22" s="6">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="Q22" s="6">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="R22" s="6">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="T22" s="6">
-        <v>33</v>
+        <v>45</v>
       </c>
       <c r="U22" s="6">
         <v>50</v>
-      </c>
-      <c r="W22" s="6">
-        <v>31</v>
-      </c>
-      <c r="X22" s="6">
-        <v>44</v>
       </c>
     </row>
   </sheetData>
@@ -2734,34 +2507,24 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="20.7109375" customWidth="1"/>
-    <col min="2" max="9" width="12.7109375" customWidth="1"/>
+    <col min="2" max="6" width="12.7109375" customWidth="1"/>
     <col min="4" max="4" width="0.85546875" customWidth="1"/>
-    <col min="7" max="7" width="0.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:61">
-      <c r="B1" s="25" t="s">
+      <c r="B1" s="23" t="s">
+        <v>40</v>
+      </c>
+      <c r="C1" s="24" t="s">
+        <v>41</v>
+      </c>
+      <c r="E1" s="25" t="s">
         <v>42</v>
       </c>
-      <c r="C1" s="26" t="s">
+      <c r="F1" s="26" t="s">
         <v>43</v>
       </c>
-      <c r="E1" s="27" t="s">
-        <v>44</v>
-      </c>
-      <c r="F1" s="28" t="s">
-        <v>45</v>
-      </c>
-      <c r="H1" s="29" t="s">
-        <v>46</v>
-      </c>
-      <c r="I1" s="30" t="s">
-        <v>47</v>
-      </c>
       <c r="M1" t="s">
-        <v>23</v>
-      </c>
-      <c r="V1" t="s">
         <v>23</v>
       </c>
       <c r="BI1" t="s">
@@ -2773,22 +2536,16 @@
         <v>0</v>
       </c>
       <c r="B2" s="4">
-        <v>0.516153796769241</v>
+        <v>0.600576779884644</v>
       </c>
       <c r="C2" s="4">
-        <v>0.483846203230759</v>
+        <v>0.399423220115356</v>
       </c>
       <c r="E2" s="4">
-        <v>0.560839687832062</v>
+        <v>0.519583796083241</v>
       </c>
       <c r="F2" s="4">
-        <v>0.439160312167938</v>
-      </c>
-      <c r="H2" s="4">
-        <v>0.420755015848997</v>
-      </c>
-      <c r="I2" s="4">
-        <v>0.579244984151003</v>
+        <v>0.480416203916759</v>
       </c>
     </row>
     <row r="3" spans="1:61">
@@ -2796,22 +2553,16 @@
         <v>1</v>
       </c>
       <c r="B3" s="5">
-        <v>27.161584767683</v>
+        <v>24.7346722530656</v>
       </c>
       <c r="C3" s="5">
-        <v>26.4145447170911</v>
+        <v>20.5730702853859</v>
       </c>
       <c r="E3" s="5">
-        <v>34.2861857427629</v>
+        <v>29.4222493155501</v>
       </c>
       <c r="F3" s="5">
-        <v>31.174044965191</v>
-      </c>
-      <c r="H3" s="5">
-        <v>18.6588144682371</v>
-      </c>
-      <c r="I3" s="5">
-        <v>21.9077028184594</v>
+        <v>28.4855795028841</v>
       </c>
     </row>
     <row r="4" spans="1:61">
@@ -2822,19 +2573,13 @@
         <v>7</v>
       </c>
       <c r="C4" s="6">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E4" s="6">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="F4" s="6">
-        <v>10</v>
-      </c>
-      <c r="H4" s="6">
-        <v>0</v>
-      </c>
-      <c r="I4" s="6">
-        <v>6</v>
+        <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:61">
@@ -2845,19 +2590,13 @@
         <v>10</v>
       </c>
       <c r="C5" s="6">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="E5" s="6">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="F5" s="6">
-        <v>14</v>
-      </c>
-      <c r="H5" s="6">
-        <v>7</v>
-      </c>
-      <c r="I5" s="6">
-        <v>7</v>
+        <v>13</v>
       </c>
     </row>
     <row r="6" spans="1:61">
@@ -2865,22 +2604,16 @@
         <v>4</v>
       </c>
       <c r="B6" s="6">
+        <v>13</v>
+      </c>
+      <c r="C6" s="6">
+        <v>10</v>
+      </c>
+      <c r="E6" s="6">
+        <v>16</v>
+      </c>
+      <c r="F6" s="6">
         <v>14</v>
-      </c>
-      <c r="C6" s="6">
-        <v>13</v>
-      </c>
-      <c r="E6" s="6">
-        <v>20</v>
-      </c>
-      <c r="F6" s="6">
-        <v>17</v>
-      </c>
-      <c r="H6" s="6">
-        <v>7</v>
-      </c>
-      <c r="I6" s="6">
-        <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:61">
@@ -2888,22 +2621,16 @@
         <v>5</v>
       </c>
       <c r="B7" s="6">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C7" s="6">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E7" s="6">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="F7" s="6">
-        <v>20</v>
-      </c>
-      <c r="H7" s="6">
-        <v>7</v>
-      </c>
-      <c r="I7" s="6">
-        <v>12</v>
+        <v>17</v>
       </c>
     </row>
     <row r="8" spans="1:61">
@@ -2911,22 +2638,16 @@
         <v>6</v>
       </c>
       <c r="B8" s="6">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C8" s="6">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="E8" s="6">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="F8" s="6">
-        <v>21</v>
-      </c>
-      <c r="H8" s="6">
-        <v>9</v>
-      </c>
-      <c r="I8" s="6">
-        <v>14</v>
+        <v>20</v>
       </c>
     </row>
     <row r="9" spans="1:61">
@@ -2934,22 +2655,16 @@
         <v>7</v>
       </c>
       <c r="B9" s="6">
+        <v>17</v>
+      </c>
+      <c r="C9" s="6">
+        <v>14</v>
+      </c>
+      <c r="E9" s="6">
+        <v>21</v>
+      </c>
+      <c r="F9" s="6">
         <v>20</v>
-      </c>
-      <c r="C9" s="6">
-        <v>19</v>
-      </c>
-      <c r="E9" s="6">
-        <v>26</v>
-      </c>
-      <c r="F9" s="6">
-        <v>23</v>
-      </c>
-      <c r="H9" s="6">
-        <v>14</v>
-      </c>
-      <c r="I9" s="6">
-        <v>15</v>
       </c>
     </row>
     <row r="10" spans="1:61">
@@ -2957,22 +2672,16 @@
         <v>8</v>
       </c>
       <c r="B10" s="6">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C10" s="6">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="E10" s="6">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="F10" s="6">
-        <v>24</v>
-      </c>
-      <c r="H10" s="6">
-        <v>14</v>
-      </c>
-      <c r="I10" s="6">
-        <v>17</v>
+        <v>23</v>
       </c>
     </row>
     <row r="11" spans="1:61">
@@ -2980,22 +2689,16 @@
         <v>9</v>
       </c>
       <c r="B11" s="6">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C11" s="6">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="E11" s="6">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="F11" s="6">
-        <v>27</v>
-      </c>
-      <c r="H11" s="6">
-        <v>14</v>
-      </c>
-      <c r="I11" s="6">
-        <v>17</v>
+        <v>24</v>
       </c>
     </row>
     <row r="12" spans="1:61">
@@ -3003,22 +2706,16 @@
         <v>10</v>
       </c>
       <c r="B12" s="6">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C12" s="6">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="E12" s="6">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="F12" s="6">
-        <v>28</v>
-      </c>
-      <c r="H12" s="6">
-        <v>14</v>
-      </c>
-      <c r="I12" s="6">
-        <v>20</v>
+        <v>26</v>
       </c>
     </row>
     <row r="13" spans="1:61">
@@ -3026,22 +2723,16 @@
         <v>11</v>
       </c>
       <c r="B13" s="6">
+        <v>24</v>
+      </c>
+      <c r="C13" s="6">
+        <v>20</v>
+      </c>
+      <c r="E13" s="6">
+        <v>28</v>
+      </c>
+      <c r="F13" s="6">
         <v>27</v>
-      </c>
-      <c r="C13" s="6">
-        <v>25</v>
-      </c>
-      <c r="E13" s="6">
-        <v>34</v>
-      </c>
-      <c r="F13" s="6">
-        <v>30</v>
-      </c>
-      <c r="H13" s="6">
-        <v>17</v>
-      </c>
-      <c r="I13" s="6">
-        <v>21</v>
       </c>
     </row>
     <row r="14" spans="1:61">
@@ -3049,22 +2740,16 @@
         <v>12</v>
       </c>
       <c r="B14" s="6">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C14" s="6">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="E14" s="6">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="F14" s="6">
-        <v>31</v>
-      </c>
-      <c r="H14" s="6">
-        <v>21</v>
-      </c>
-      <c r="I14" s="6">
-        <v>23</v>
+        <v>29</v>
       </c>
     </row>
     <row r="15" spans="1:61">
@@ -3072,22 +2757,16 @@
         <v>13</v>
       </c>
       <c r="B15" s="6">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="C15" s="6">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="E15" s="6">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="F15" s="6">
-        <v>34</v>
-      </c>
-      <c r="H15" s="6">
-        <v>21</v>
-      </c>
-      <c r="I15" s="6">
-        <v>24</v>
+        <v>31</v>
       </c>
     </row>
     <row r="16" spans="1:61">
@@ -3095,160 +2774,118 @@
         <v>14</v>
       </c>
       <c r="B16" s="6">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C16" s="6">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="E16" s="6">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="F16" s="6">
-        <v>35</v>
-      </c>
-      <c r="H16" s="6">
-        <v>21</v>
-      </c>
-      <c r="I16" s="6">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
       <c r="A17" s="3" t="s">
         <v>15</v>
       </c>
       <c r="B17" s="6">
+        <v>30</v>
+      </c>
+      <c r="C17" s="6">
+        <v>26</v>
+      </c>
+      <c r="E17" s="6">
+        <v>36</v>
+      </c>
+      <c r="F17" s="6">
         <v>34</v>
       </c>
-      <c r="C17" s="6">
-        <v>32</v>
-      </c>
-      <c r="E17" s="6">
-        <v>41</v>
-      </c>
-      <c r="F17" s="6">
-        <v>38</v>
-      </c>
-      <c r="H17" s="6">
-        <v>22</v>
-      </c>
-      <c r="I17" s="6">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9">
+    </row>
+    <row r="18" spans="1:6">
       <c r="A18" s="3" t="s">
         <v>16</v>
       </c>
       <c r="B18" s="6">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C18" s="6">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="E18" s="6">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="F18" s="6">
-        <v>40</v>
-      </c>
-      <c r="H18" s="6">
-        <v>27</v>
-      </c>
-      <c r="I18" s="6">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6">
       <c r="A19" s="3" t="s">
         <v>17</v>
       </c>
       <c r="B19" s="6">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="C19" s="6">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="E19" s="6">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="F19" s="6">
-        <v>43</v>
-      </c>
-      <c r="H19" s="6">
-        <v>28</v>
-      </c>
-      <c r="I19" s="6">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6">
       <c r="A20" s="3" t="s">
         <v>18</v>
       </c>
       <c r="B20" s="6">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="C20" s="6">
-        <v>40</v>
+        <v>31</v>
       </c>
       <c r="E20" s="6">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="F20" s="6">
-        <v>45</v>
-      </c>
-      <c r="H20" s="6">
-        <v>29</v>
-      </c>
-      <c r="I20" s="6">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6">
       <c r="A21" s="3" t="s">
         <v>19</v>
       </c>
       <c r="B21" s="6">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="C21" s="6">
-        <v>44</v>
+        <v>34</v>
       </c>
       <c r="E21" s="6">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="F21" s="6">
-        <v>50</v>
-      </c>
-      <c r="H21" s="6">
-        <v>35</v>
-      </c>
-      <c r="I21" s="6">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6">
       <c r="A22" s="3" t="s">
         <v>20</v>
       </c>
       <c r="B22" s="6">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="C22" s="6">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="E22" s="6">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="F22" s="6">
-        <v>56</v>
-      </c>
-      <c r="H22" s="6">
-        <v>41</v>
-      </c>
-      <c r="I22" s="6">
-        <v>43</v>
+        <v>52</v>
       </c>
     </row>
   </sheetData>
@@ -3272,11 +2909,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:61">
-      <c r="B1" s="31" t="s">
-        <v>48</v>
-      </c>
-      <c r="C1" s="32" t="s">
-        <v>49</v>
+      <c r="B1" s="27" t="s">
+        <v>44</v>
+      </c>
+      <c r="C1" s="28" t="s">
+        <v>45</v>
       </c>
       <c r="BI1" t="s">
         <v>23</v>
@@ -3287,10 +2924,10 @@
         <v>0</v>
       </c>
       <c r="B2" s="4">
-        <v>0.591590881681824</v>
+        <v>0.421200615759877</v>
       </c>
       <c r="C2" s="4">
-        <v>0.408409118318176</v>
+        <v>0.578799384240123</v>
       </c>
     </row>
     <row r="3" spans="1:61">
@@ -3298,10 +2935,10 @@
         <v>1</v>
       </c>
       <c r="B3" s="5">
-        <v>18.4520187095963</v>
+        <v>18.9618090076382</v>
       </c>
       <c r="C3" s="5">
-        <v>15.1470775705845</v>
+        <v>22.1710217657956</v>
       </c>
     </row>
     <row r="4" spans="1:61">
@@ -3312,7 +2949,7 @@
         <v>3</v>
       </c>
       <c r="C4" s="6">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:61">
@@ -3320,10 +2957,10 @@
         <v>3</v>
       </c>
       <c r="B5" s="6">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C5" s="6">
-        <v>3</v>
+        <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:61">
@@ -3334,7 +2971,7 @@
         <v>7</v>
       </c>
       <c r="C6" s="6">
-        <v>6</v>
+        <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:61">
@@ -3342,10 +2979,10 @@
         <v>5</v>
       </c>
       <c r="B7" s="6">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C7" s="6">
-        <v>7</v>
+        <v>13</v>
       </c>
     </row>
     <row r="8" spans="1:61">
@@ -3356,7 +2993,7 @@
         <v>10</v>
       </c>
       <c r="C8" s="6">
-        <v>9</v>
+        <v>14</v>
       </c>
     </row>
     <row r="9" spans="1:61">
@@ -3364,10 +3001,10 @@
         <v>7</v>
       </c>
       <c r="B9" s="6">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C9" s="6">
-        <v>10</v>
+        <v>16</v>
       </c>
     </row>
     <row r="10" spans="1:61">
@@ -3378,7 +3015,7 @@
         <v>14</v>
       </c>
       <c r="C10" s="6">
-        <v>10</v>
+        <v>17</v>
       </c>
     </row>
     <row r="11" spans="1:61">
@@ -3389,7 +3026,7 @@
         <v>14</v>
       </c>
       <c r="C11" s="6">
-        <v>12</v>
+        <v>19</v>
       </c>
     </row>
     <row r="12" spans="1:61">
@@ -3397,10 +3034,10 @@
         <v>10</v>
       </c>
       <c r="B12" s="6">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C12" s="6">
-        <v>13</v>
+        <v>20</v>
       </c>
     </row>
     <row r="13" spans="1:61">
@@ -3411,7 +3048,7 @@
         <v>17</v>
       </c>
       <c r="C13" s="6">
-        <v>14</v>
+        <v>21</v>
       </c>
     </row>
     <row r="14" spans="1:61">
@@ -3419,10 +3056,10 @@
         <v>12</v>
       </c>
       <c r="B14" s="6">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C14" s="6">
-        <v>16</v>
+        <v>23</v>
       </c>
     </row>
     <row r="15" spans="1:61">
@@ -3430,10 +3067,10 @@
         <v>13</v>
       </c>
       <c r="B15" s="6">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C15" s="6">
-        <v>16</v>
+        <v>24</v>
       </c>
     </row>
     <row r="16" spans="1:61">
@@ -3441,10 +3078,10 @@
         <v>14</v>
       </c>
       <c r="B16" s="6">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C16" s="6">
-        <v>17</v>
+        <v>26</v>
       </c>
     </row>
     <row r="17" spans="1:3">
@@ -3452,10 +3089,10 @@
         <v>15</v>
       </c>
       <c r="B17" s="6">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C17" s="6">
-        <v>19</v>
+        <v>27</v>
       </c>
     </row>
     <row r="18" spans="1:3">
@@ -3463,10 +3100,10 @@
         <v>16</v>
       </c>
       <c r="B18" s="6">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C18" s="6">
-        <v>20</v>
+        <v>29</v>
       </c>
     </row>
     <row r="19" spans="1:3">
@@ -3474,10 +3111,10 @@
         <v>17</v>
       </c>
       <c r="B19" s="6">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C19" s="6">
-        <v>23</v>
+        <v>31</v>
       </c>
     </row>
     <row r="20" spans="1:3">
@@ -3485,10 +3122,10 @@
         <v>18</v>
       </c>
       <c r="B20" s="6">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C20" s="6">
-        <v>24</v>
+        <v>34</v>
       </c>
     </row>
     <row r="21" spans="1:3">
@@ -3496,10 +3133,10 @@
         <v>19</v>
       </c>
       <c r="B21" s="6">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C21" s="6">
-        <v>27</v>
+        <v>37</v>
       </c>
     </row>
     <row r="22" spans="1:3">
@@ -3510,7 +3147,7 @@
         <v>38</v>
       </c>
       <c r="C22" s="6">
-        <v>32</v>
+        <v>43</v>
       </c>
     </row>
   </sheetData>
@@ -3534,11 +3171,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:61">
-      <c r="B1" s="33" t="s">
-        <v>50</v>
-      </c>
-      <c r="C1" s="34" t="s">
-        <v>51</v>
+      <c r="B1" s="29" t="s">
+        <v>46</v>
+      </c>
+      <c r="C1" s="30" t="s">
+        <v>47</v>
       </c>
       <c r="BI1" t="s">
         <v>23</v>
@@ -3549,10 +3186,10 @@
         <v>0</v>
       </c>
       <c r="B2" s="4">
-        <v>0.532325393534921</v>
+        <v>0.134101573179685</v>
       </c>
       <c r="C2" s="4">
-        <v>0.467674606465079</v>
+        <v>0.865898426820315</v>
       </c>
     </row>
     <row r="3" spans="1:61">
@@ -3560,10 +3197,10 @@
         <v>1</v>
       </c>
       <c r="B3" s="5">
-        <v>17.2256679548664</v>
+        <v>8.0060669987866</v>
       </c>
       <c r="C3" s="5">
-        <v>16.1249119750176</v>
+        <v>22.6752152649569</v>
       </c>
     </row>
     <row r="4" spans="1:61">
@@ -3571,10 +3208,10 @@
         <v>2</v>
       </c>
       <c r="B4" s="6">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="C4" s="6">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:61">
@@ -3582,10 +3219,10 @@
         <v>3</v>
       </c>
       <c r="B5" s="6">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="C5" s="6">
-        <v>6</v>
+        <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:61">
@@ -3593,10 +3230,10 @@
         <v>4</v>
       </c>
       <c r="B6" s="6">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="C6" s="6">
-        <v>6</v>
+        <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:61">
@@ -3604,10 +3241,10 @@
         <v>5</v>
       </c>
       <c r="B7" s="6">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="C7" s="6">
-        <v>9</v>
+        <v>13</v>
       </c>
     </row>
     <row r="8" spans="1:61">
@@ -3615,10 +3252,10 @@
         <v>6</v>
       </c>
       <c r="B8" s="6">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="C8" s="6">
-        <v>10</v>
+        <v>14</v>
       </c>
     </row>
     <row r="9" spans="1:61">
@@ -3626,10 +3263,10 @@
         <v>7</v>
       </c>
       <c r="B9" s="6">
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="C9" s="6">
-        <v>10</v>
+        <v>16</v>
       </c>
     </row>
     <row r="10" spans="1:61">
@@ -3637,10 +3274,10 @@
         <v>8</v>
       </c>
       <c r="B10" s="6">
-        <v>13</v>
+        <v>3</v>
       </c>
       <c r="C10" s="6">
-        <v>12</v>
+        <v>17</v>
       </c>
     </row>
     <row r="11" spans="1:61">
@@ -3648,10 +3285,10 @@
         <v>9</v>
       </c>
       <c r="B11" s="6">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="C11" s="6">
-        <v>13</v>
+        <v>19</v>
       </c>
     </row>
     <row r="12" spans="1:61">
@@ -3659,10 +3296,10 @@
         <v>10</v>
       </c>
       <c r="B12" s="6">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="C12" s="6">
-        <v>13</v>
+        <v>20</v>
       </c>
     </row>
     <row r="13" spans="1:61">
@@ -3670,10 +3307,10 @@
         <v>11</v>
       </c>
       <c r="B13" s="6">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="C13" s="6">
-        <v>16</v>
+        <v>22</v>
       </c>
     </row>
     <row r="14" spans="1:61">
@@ -3681,10 +3318,10 @@
         <v>12</v>
       </c>
       <c r="B14" s="6">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="C14" s="6">
-        <v>16</v>
+        <v>23</v>
       </c>
     </row>
     <row r="15" spans="1:61">
@@ -3692,10 +3329,10 @@
         <v>13</v>
       </c>
       <c r="B15" s="6">
-        <v>19</v>
+        <v>8</v>
       </c>
       <c r="C15" s="6">
-        <v>17</v>
+        <v>24</v>
       </c>
     </row>
     <row r="16" spans="1:61">
@@ -3703,10 +3340,10 @@
         <v>14</v>
       </c>
       <c r="B16" s="6">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="C16" s="6">
-        <v>19</v>
+        <v>26</v>
       </c>
     </row>
     <row r="17" spans="1:3">
@@ -3714,10 +3351,10 @@
         <v>15</v>
       </c>
       <c r="B17" s="6">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="C17" s="6">
-        <v>20</v>
+        <v>28</v>
       </c>
     </row>
     <row r="18" spans="1:3">
@@ -3725,10 +3362,10 @@
         <v>16</v>
       </c>
       <c r="B18" s="6">
-        <v>23</v>
+        <v>13</v>
       </c>
       <c r="C18" s="6">
-        <v>22</v>
+        <v>30</v>
       </c>
     </row>
     <row r="19" spans="1:3">
@@ -3736,10 +3373,10 @@
         <v>17</v>
       </c>
       <c r="B19" s="6">
-        <v>25</v>
+        <v>14</v>
       </c>
       <c r="C19" s="6">
-        <v>23</v>
+        <v>32</v>
       </c>
     </row>
     <row r="20" spans="1:3">
@@ -3747,10 +3384,10 @@
         <v>18</v>
       </c>
       <c r="B20" s="6">
-        <v>27</v>
+        <v>14</v>
       </c>
       <c r="C20" s="6">
-        <v>26</v>
+        <v>35</v>
       </c>
     </row>
     <row r="21" spans="1:3">
@@ -3758,10 +3395,10 @@
         <v>19</v>
       </c>
       <c r="B21" s="6">
-        <v>30</v>
+        <v>17</v>
       </c>
       <c r="C21" s="6">
-        <v>29</v>
+        <v>38</v>
       </c>
     </row>
     <row r="22" spans="1:3">
@@ -3769,10 +3406,10 @@
         <v>20</v>
       </c>
       <c r="B22" s="6">
-        <v>34</v>
+        <v>21</v>
       </c>
       <c r="C22" s="6">
-        <v>33</v>
+        <v>43</v>
       </c>
     </row>
   </sheetData>

</xml_diff>